<commit_message>
updates and last update to folder
</commit_message>
<xml_diff>
--- a/Qualitydata_Decomposition_BF3.xlsx
+++ b/Qualitydata_Decomposition_BF3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hirsc\OneDrive\Documents\ExperimentalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4ECB40-6AAB-48EB-859A-A88BE1688BE5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E8821F-F5B9-40DF-891A-2ADD69F1AD46}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,11 +579,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -908,7 +908,7 @@
   <dimension ref="A1:AZ19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AW11" sqref="AW11"/>
+      <selection activeCell="AW12" sqref="AW12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,12 +937,12 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
       <c r="I1" t="s">
         <v>4</v>
       </c>
@@ -990,134 +990,134 @@
       <c r="G2">
         <v>122.6</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <f>AVERAGE($D$2:$G$9)</f>
         <v>95.146875000000009</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <f t="shared" ref="J2:L2" si="0">AVERAGE($D$2:$G$9)</f>
         <v>95.146875000000009</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <f t="shared" si="0"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <f t="shared" si="0"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1">
         <f>AVERAGE($D$2:$G$5)</f>
         <v>110.72500000000001</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <f t="shared" ref="O2:Q5" si="1">AVERAGE($D$2:$G$5)</f>
         <v>110.72500000000001</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1">
         <f>AVERAGE($D$2:$G$3,$D$6:$G$7)</f>
         <v>101.24999999999999</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <f t="shared" ref="T2:V3" si="2">AVERAGE($D$2:$G$3,$D$6:$G$7)</f>
         <v>101.24999999999999</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <f t="shared" si="2"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <f t="shared" si="2"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2">
+      <c r="W2" s="1"/>
+      <c r="X2" s="1">
         <f>AVERAGE($D$2:$G$2,$D$4:$G$4,$D$6:$G$6,$D$8:$G$8)</f>
         <v>104.0625</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="1">
         <f t="shared" ref="Y2:AA8" si="3">AVERAGE($D$2:$G$2,$D$4:$G$4,$D$6:$G$6,$D$8:$G$8)</f>
         <v>104.0625</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="1">
         <f>AVERAGE($D$2:$G$3)</f>
         <v>116.65</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="1">
         <f t="shared" ref="AD2:AF3" si="4">AVERAGE($D$2:$G$3)</f>
         <v>116.65</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE2" s="1">
         <f t="shared" si="4"/>
         <v>116.65</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AF2" s="1">
         <f t="shared" si="4"/>
         <v>116.65</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AH2" s="1">
         <f>AVERAGE($D$2:$G$2,$D$4:$G$4)</f>
         <v>119.48749999999998</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2" s="1">
         <f t="shared" ref="AI2:AK2" si="5">AVERAGE($D$2:$G$2,$D$4:$G$4)</f>
         <v>119.48749999999998</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AJ2" s="1">
         <f t="shared" si="5"/>
         <v>119.48749999999998</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AK2" s="1">
         <f t="shared" si="5"/>
         <v>119.48749999999998</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AM2" s="1">
         <f>AVERAGE($D$2:$G$2,$D$6:$G$6)</f>
         <v>106.89999999999998</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AN2" s="1">
         <f t="shared" ref="AN2:AP2" si="6">AVERAGE($D$2:$G$2,$D$6:$G$6)</f>
         <v>106.89999999999998</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AO2" s="1">
         <f t="shared" si="6"/>
         <v>106.89999999999998</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="AP2" s="1">
         <f t="shared" si="6"/>
         <v>106.89999999999998</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AR2" s="1">
         <f>AVERAGE($D2:$G2)</f>
         <v>122.04999999999998</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AS2" s="1">
         <f t="shared" ref="AS2:AU9" si="7">AVERAGE($D2:$G2)</f>
         <v>122.04999999999998</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AT2" s="1">
         <f t="shared" si="7"/>
         <v>122.04999999999998</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="AU2" s="1">
         <f t="shared" si="7"/>
         <v>122.04999999999998</v>
       </c>
@@ -1144,134 +1144,134 @@
       <c r="G3">
         <v>108.6</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f t="shared" ref="I3:L9" si="8">AVERAGE($D$2:$G$9)</f>
         <v>95.146875000000009</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1">
         <f t="shared" ref="N3:N5" si="9">AVERAGE($D$2:$G$5)</f>
         <v>110.72500000000001</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1">
         <f>AVERAGE($D$2:$G$3,$D$6:$G$7)</f>
         <v>101.24999999999999</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="1">
         <f t="shared" si="2"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="1">
         <f t="shared" si="2"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="1">
         <f t="shared" si="2"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2">
+      <c r="W3" s="1"/>
+      <c r="X3" s="1">
         <f>AVERAGE($D$3:$G$3,$D$5:$G$5,$D$7:$G$7,$D$9:$G$9)</f>
         <v>86.231249999999989</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3" s="1">
         <f t="shared" ref="Y3:AA9" si="10">AVERAGE($D$3:$G$3,$D$5:$G$5,$D$7:$G$7,$D$9:$G$9)</f>
         <v>86.231249999999989</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AC3" s="1">
         <f>AVERAGE($D$2:$G$3)</f>
         <v>116.65</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3" s="1">
         <f t="shared" si="4"/>
         <v>116.65</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AE3" s="1">
         <f t="shared" si="4"/>
         <v>116.65</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF3" s="1">
         <f t="shared" si="4"/>
         <v>116.65</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AH3" s="1">
         <f>AVERAGE($D$3:$G$3,$D$5:$G$5)</f>
         <v>101.96250000000001</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI3" s="1">
         <f t="shared" ref="AI3:AK3" si="11">AVERAGE($D$3:$G$3,$D$5:$G$5)</f>
         <v>101.96250000000001</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="AJ3" s="1">
         <f t="shared" si="11"/>
         <v>101.96250000000001</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="AK3" s="1">
         <f t="shared" si="11"/>
         <v>101.96250000000001</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="AM3" s="1">
         <f>AVERAGE($D$3:$G$3,$D$7:$G$7)</f>
         <v>95.600000000000009</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="AN3" s="1">
         <f t="shared" ref="AN3:AP3" si="12">AVERAGE($D$3:$G$3,$D$7:$G$7)</f>
         <v>95.600000000000009</v>
       </c>
-      <c r="AO3" s="2">
+      <c r="AO3" s="1">
         <f t="shared" si="12"/>
         <v>95.600000000000009</v>
       </c>
-      <c r="AP3" s="2">
+      <c r="AP3" s="1">
         <f t="shared" si="12"/>
         <v>95.600000000000009</v>
       </c>
-      <c r="AR3" s="2">
+      <c r="AR3" s="1">
         <f t="shared" ref="AR3:AR9" si="13">AVERAGE($D3:$G3)</f>
         <v>111.25</v>
       </c>
-      <c r="AS3" s="2">
+      <c r="AS3" s="1">
         <f t="shared" si="7"/>
         <v>111.25</v>
       </c>
-      <c r="AT3" s="2">
+      <c r="AT3" s="1">
         <f t="shared" si="7"/>
         <v>111.25</v>
       </c>
-      <c r="AU3" s="2">
+      <c r="AU3" s="1">
         <f t="shared" si="7"/>
         <v>111.25</v>
       </c>
@@ -1298,134 +1298,134 @@
       <c r="G4">
         <v>117.3</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
         <f t="shared" si="9"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1">
         <f>AVERAGE($D$4:$G$5,$D$8:$G$9)</f>
         <v>89.043749999999989</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <f t="shared" ref="T4:V5" si="14">AVERAGE($D$4:$G$5,$D$8:$G$9)</f>
         <v>89.043749999999989</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="1">
         <f t="shared" si="14"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="1">
         <f t="shared" si="14"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2">
+      <c r="W4" s="1"/>
+      <c r="X4" s="1">
         <f>AVERAGE($D$2:$G$2,$D$4:$G$4,$D$6:$G$6,$D$8:$G$8)</f>
         <v>104.0625</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC4" s="1">
         <f>AVERAGE($D$4:$G$5)</f>
         <v>104.8</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="1">
         <f t="shared" ref="AD4:AF5" si="15">AVERAGE($D$4:$G$5)</f>
         <v>104.8</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE4" s="1">
         <f t="shared" si="15"/>
         <v>104.8</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AF4" s="1">
         <f t="shared" si="15"/>
         <v>104.8</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="AH4" s="1">
         <f>AVERAGE($D$2:$G$2,$D$4:$G$4)</f>
         <v>119.48749999999998</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AI4" s="1">
         <f t="shared" ref="AI4:AK4" si="16">AVERAGE($D$2:$G$2,$D$4:$G$4)</f>
         <v>119.48749999999998</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="AJ4" s="1">
         <f t="shared" si="16"/>
         <v>119.48749999999998</v>
       </c>
-      <c r="AK4" s="2">
+      <c r="AK4" s="1">
         <f t="shared" si="16"/>
         <v>119.48749999999998</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="AM4" s="1">
         <f>AVERAGE($D$4:$G$4,$D$8:$G$8)</f>
         <v>101.22500000000001</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="AN4" s="1">
         <f t="shared" ref="AN4:AP4" si="17">AVERAGE($D$4:$G$4,$D$8:$G$8)</f>
         <v>101.22500000000001</v>
       </c>
-      <c r="AO4" s="2">
+      <c r="AO4" s="1">
         <f t="shared" si="17"/>
         <v>101.22500000000001</v>
       </c>
-      <c r="AP4" s="2">
+      <c r="AP4" s="1">
         <f t="shared" si="17"/>
         <v>101.22500000000001</v>
       </c>
-      <c r="AR4" s="2">
+      <c r="AR4" s="1">
         <f t="shared" si="13"/>
         <v>116.925</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AS4" s="1">
         <f t="shared" si="7"/>
         <v>116.925</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AT4" s="1">
         <f t="shared" si="7"/>
         <v>116.925</v>
       </c>
-      <c r="AU4" s="2">
+      <c r="AU4" s="1">
         <f t="shared" si="7"/>
         <v>116.925</v>
       </c>
@@ -1452,134 +1452,134 @@
       <c r="G5">
         <v>90.1</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
         <f t="shared" si="9"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <f t="shared" si="1"/>
         <v>110.72500000000001</v>
       </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2">
+      <c r="R5" s="1"/>
+      <c r="S5" s="1">
         <f>AVERAGE($D$4:$G$5,$D$8:$G$9)</f>
         <v>89.043749999999989</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="1">
         <f t="shared" si="14"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="1">
         <f t="shared" si="14"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="1">
         <f t="shared" si="14"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2">
+      <c r="W5" s="1"/>
+      <c r="X5" s="1">
         <f>AVERAGE($D$3:$G$3,$D$5:$G$5,$D$7:$G$7,$D$9:$G$9)</f>
         <v>86.231249999999989</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AA5" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AC5" s="1">
         <f>AVERAGE($D$4:$G$5)</f>
         <v>104.8</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="1">
         <f t="shared" si="15"/>
         <v>104.8</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AE5" s="1">
         <f t="shared" si="15"/>
         <v>104.8</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AF5" s="1">
         <f t="shared" si="15"/>
         <v>104.8</v>
       </c>
-      <c r="AH5" s="2">
+      <c r="AH5" s="1">
         <f>AVERAGE($D$3:$G$3,$D$5:$G$5)</f>
         <v>101.96250000000001</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AI5" s="1">
         <f t="shared" ref="AI5:AK5" si="18">AVERAGE($D$3:$G$3,$D$5:$G$5)</f>
         <v>101.96250000000001</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="AJ5" s="1">
         <f t="shared" si="18"/>
         <v>101.96250000000001</v>
       </c>
-      <c r="AK5" s="2">
+      <c r="AK5" s="1">
         <f t="shared" si="18"/>
         <v>101.96250000000001</v>
       </c>
-      <c r="AM5" s="2">
+      <c r="AM5" s="1">
         <f>AVERAGE($D$5:$G$5,$D$9:$G$9)</f>
         <v>76.862499999999997</v>
       </c>
-      <c r="AN5" s="2">
+      <c r="AN5" s="1">
         <f t="shared" ref="AN5:AP5" si="19">AVERAGE($D$5:$G$5,$D$9:$G$9)</f>
         <v>76.862499999999997</v>
       </c>
-      <c r="AO5" s="2">
+      <c r="AO5" s="1">
         <f t="shared" si="19"/>
         <v>76.862499999999997</v>
       </c>
-      <c r="AP5" s="2">
+      <c r="AP5" s="1">
         <f t="shared" si="19"/>
         <v>76.862499999999997</v>
       </c>
-      <c r="AR5" s="2">
+      <c r="AR5" s="1">
         <f t="shared" si="13"/>
         <v>92.675000000000011</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AS5" s="1">
         <f t="shared" si="7"/>
         <v>92.675000000000011</v>
       </c>
-      <c r="AT5" s="2">
+      <c r="AT5" s="1">
         <f t="shared" si="7"/>
         <v>92.675000000000011</v>
       </c>
-      <c r="AU5" s="2">
+      <c r="AU5" s="1">
         <f t="shared" si="7"/>
         <v>92.675000000000011</v>
       </c>
@@ -1606,134 +1606,134 @@
       <c r="G6">
         <v>92</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
         <f>AVERAGE($D$6:$G$9)</f>
         <v>79.568749999999994</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <f t="shared" ref="O6:Q9" si="20">AVERAGE($D$6:$G$9)</f>
         <v>79.568749999999994</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2">
+      <c r="R6" s="1"/>
+      <c r="S6" s="1">
         <f>AVERAGE($D$2:$G$3,$D$6:$G$7)</f>
         <v>101.24999999999999</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="1">
         <f t="shared" ref="T6:V7" si="21">AVERAGE($D$2:$G$3,$D$6:$G$7)</f>
         <v>101.24999999999999</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="1">
         <f t="shared" si="21"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="1">
         <f t="shared" si="21"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2">
+      <c r="W6" s="1"/>
+      <c r="X6" s="1">
         <f>AVERAGE($D$2:$G$2,$D$4:$G$4,$D$6:$G$6,$D$8:$G$8)</f>
         <v>104.0625</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA6" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AC6" s="1">
         <f>AVERAGE($D$6:$G$7)</f>
         <v>85.850000000000009</v>
       </c>
-      <c r="AD6" s="2">
-        <f t="shared" ref="AD6:AF8" si="22">AVERAGE($D$6:$G$7)</f>
+      <c r="AD6" s="1">
+        <f t="shared" ref="AD6:AF7" si="22">AVERAGE($D$6:$G$7)</f>
         <v>85.850000000000009</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AE6" s="1">
         <f t="shared" si="22"/>
         <v>85.850000000000009</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AF6" s="1">
         <f t="shared" si="22"/>
         <v>85.850000000000009</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="AH6" s="1">
         <f>AVERAGE($D$6:$G$6,$D$8:$G$8)</f>
         <v>88.637500000000003</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AI6" s="1">
         <f t="shared" ref="AI6:AK6" si="23">AVERAGE($D$6:$G$6,$D$8:$G$8)</f>
         <v>88.637500000000003</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="AJ6" s="1">
         <f t="shared" si="23"/>
         <v>88.637500000000003</v>
       </c>
-      <c r="AK6" s="2">
+      <c r="AK6" s="1">
         <f t="shared" si="23"/>
         <v>88.637500000000003</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="AM6" s="1">
         <f>AVERAGE($D$2:$G$2,$D$6:$G$6)</f>
         <v>106.89999999999998</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="AN6" s="1">
         <f t="shared" ref="AN6:AP6" si="24">AVERAGE($D$2:$G$2,$D$6:$G$6)</f>
         <v>106.89999999999998</v>
       </c>
-      <c r="AO6" s="2">
+      <c r="AO6" s="1">
         <f t="shared" si="24"/>
         <v>106.89999999999998</v>
       </c>
-      <c r="AP6" s="2">
+      <c r="AP6" s="1">
         <f t="shared" si="24"/>
         <v>106.89999999999998</v>
       </c>
-      <c r="AR6" s="2">
+      <c r="AR6" s="1">
         <f t="shared" si="13"/>
         <v>91.75</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AS6" s="1">
         <f t="shared" si="7"/>
         <v>91.75</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AT6" s="1">
         <f t="shared" si="7"/>
         <v>91.75</v>
       </c>
-      <c r="AU6" s="2">
+      <c r="AU6" s="1">
         <f t="shared" si="7"/>
         <v>91.75</v>
       </c>
@@ -1760,134 +1760,134 @@
       <c r="G7">
         <v>77.099999999999994</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2">
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
         <f t="shared" ref="N7:N9" si="25">AVERAGE($D$6:$G$9)</f>
         <v>79.568749999999994</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2">
+      <c r="R7" s="1"/>
+      <c r="S7" s="1">
         <f>AVERAGE($D$2:$G$3,$D$6:$G$7)</f>
         <v>101.24999999999999</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="1">
         <f t="shared" si="21"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="1">
         <f t="shared" si="21"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="1">
         <f t="shared" si="21"/>
         <v>101.24999999999999</v>
       </c>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2">
+      <c r="W7" s="1"/>
+      <c r="X7" s="1">
         <f>AVERAGE($D$3:$G$3,$D$5:$G$5,$D$7:$G$7,$D$9:$G$9)</f>
         <v>86.231249999999989</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Y7" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="Z7" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AA7" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AC7" s="2">
-        <f t="shared" ref="AC7:AC8" si="26">AVERAGE($D$6:$G$7)</f>
+      <c r="AC7" s="1">
+        <f t="shared" ref="AC7" si="26">AVERAGE($D$6:$G$7)</f>
         <v>85.850000000000009</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AD7" s="1">
         <f t="shared" si="22"/>
         <v>85.850000000000009</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AE7" s="1">
         <f t="shared" si="22"/>
         <v>85.850000000000009</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AF7" s="1">
         <f t="shared" si="22"/>
         <v>85.850000000000009</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AH7" s="1">
         <f>AVERAGE($D$7:$G$7,$D$9:$G$9)</f>
         <v>70.5</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AI7" s="1">
         <f t="shared" ref="AI7:AK7" si="27">AVERAGE($D$7:$G$7,$D$9:$G$9)</f>
         <v>70.5</v>
       </c>
-      <c r="AJ7" s="2">
+      <c r="AJ7" s="1">
         <f t="shared" si="27"/>
         <v>70.5</v>
       </c>
-      <c r="AK7" s="2">
+      <c r="AK7" s="1">
         <f t="shared" si="27"/>
         <v>70.5</v>
       </c>
-      <c r="AM7" s="2">
+      <c r="AM7" s="1">
         <f>AVERAGE($D$3:$G$3,$D$7:$G$7)</f>
         <v>95.600000000000009</v>
       </c>
-      <c r="AN7" s="2">
+      <c r="AN7" s="1">
         <f t="shared" ref="AN7:AP7" si="28">AVERAGE($D$3:$G$3,$D$7:$G$7)</f>
         <v>95.600000000000009</v>
       </c>
-      <c r="AO7" s="2">
+      <c r="AO7" s="1">
         <f t="shared" si="28"/>
         <v>95.600000000000009</v>
       </c>
-      <c r="AP7" s="2">
+      <c r="AP7" s="1">
         <f t="shared" si="28"/>
         <v>95.600000000000009</v>
       </c>
-      <c r="AR7" s="2">
+      <c r="AR7" s="1">
         <f t="shared" si="13"/>
         <v>79.949999999999989</v>
       </c>
-      <c r="AS7" s="2">
+      <c r="AS7" s="1">
         <f t="shared" si="7"/>
         <v>79.949999999999989</v>
       </c>
-      <c r="AT7" s="2">
+      <c r="AT7" s="1">
         <f t="shared" si="7"/>
         <v>79.949999999999989</v>
       </c>
-      <c r="AU7" s="2">
+      <c r="AU7" s="1">
         <f t="shared" si="7"/>
         <v>79.949999999999989</v>
       </c>
@@ -1914,134 +1914,134 @@
       <c r="G8">
         <v>82.7</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1">
         <f t="shared" si="25"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2">
+      <c r="R8" s="1"/>
+      <c r="S8" s="1">
         <f>AVERAGE($D$4:$G$5,$D$8:$G$9)</f>
         <v>89.043749999999989</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="1">
         <f t="shared" ref="T8:V9" si="29">AVERAGE($D$4:$G$5,$D$8:$G$9)</f>
         <v>89.043749999999989</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="1">
         <f t="shared" si="29"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="1">
         <f t="shared" si="29"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2">
+      <c r="W8" s="1"/>
+      <c r="X8" s="1">
         <f>AVERAGE($D$2:$G$2,$D$4:$G$4,$D$6:$G$6,$D$8:$G$8)</f>
         <v>104.0625</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Y8" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="Z8" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AA8" s="1">
         <f t="shared" si="3"/>
         <v>104.0625</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AC8" s="1">
         <f>AVERAGE($D$8:$G$9)</f>
         <v>73.287499999999994</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8" s="1">
         <f t="shared" ref="AD8:AF9" si="30">AVERAGE($D$8:$G$9)</f>
         <v>73.287499999999994</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AE8" s="1">
         <f t="shared" si="30"/>
         <v>73.287499999999994</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AF8" s="1">
         <f t="shared" si="30"/>
         <v>73.287499999999994</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AH8" s="1">
         <f>AVERAGE($D$6:$G$6,$D$8:$G$8)</f>
         <v>88.637500000000003</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AI8" s="1">
         <f t="shared" ref="AI8:AK8" si="31">AVERAGE($D$6:$G$6,$D$8:$G$8)</f>
         <v>88.637500000000003</v>
       </c>
-      <c r="AJ8" s="2">
+      <c r="AJ8" s="1">
         <f t="shared" si="31"/>
         <v>88.637500000000003</v>
       </c>
-      <c r="AK8" s="2">
+      <c r="AK8" s="1">
         <f t="shared" si="31"/>
         <v>88.637500000000003</v>
       </c>
-      <c r="AM8" s="2">
+      <c r="AM8" s="1">
         <f>AVERAGE($D$4:$G$4,$D$8:$G$8)</f>
         <v>101.22500000000001</v>
       </c>
-      <c r="AN8" s="2">
+      <c r="AN8" s="1">
         <f t="shared" ref="AN8:AP8" si="32">AVERAGE($D$4:$G$4,$D$8:$G$8)</f>
         <v>101.22500000000001</v>
       </c>
-      <c r="AO8" s="2">
+      <c r="AO8" s="1">
         <f t="shared" si="32"/>
         <v>101.22500000000001</v>
       </c>
-      <c r="AP8" s="2">
+      <c r="AP8" s="1">
         <f t="shared" si="32"/>
         <v>101.22500000000001</v>
       </c>
-      <c r="AR8" s="2">
+      <c r="AR8" s="1">
         <f t="shared" si="13"/>
         <v>85.524999999999991</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AS8" s="1">
         <f t="shared" si="7"/>
         <v>85.524999999999991</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AT8" s="1">
         <f t="shared" si="7"/>
         <v>85.524999999999991</v>
       </c>
-      <c r="AU8" s="2">
+      <c r="AU8" s="1">
         <f t="shared" si="7"/>
         <v>85.524999999999991</v>
       </c>
@@ -2068,134 +2068,134 @@
       <c r="G9">
         <v>62.3</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <f t="shared" si="8"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1">
         <f t="shared" si="25"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="1">
         <f t="shared" si="20"/>
         <v>79.568749999999994</v>
       </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2">
+      <c r="R9" s="1"/>
+      <c r="S9" s="1">
         <f>AVERAGE($D$4:$G$5,$D$8:$G$9)</f>
         <v>89.043749999999989</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="1">
         <f t="shared" si="29"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="1">
         <f t="shared" si="29"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9" s="1">
         <f t="shared" si="29"/>
         <v>89.043749999999989</v>
       </c>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2">
+      <c r="W9" s="1"/>
+      <c r="X9" s="1">
         <f>AVERAGE($D$3:$G$3,$D$5:$G$5,$D$7:$G$7,$D$9:$G$9)</f>
         <v>86.231249999999989</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Y9" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Z9" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AA9" s="1">
         <f t="shared" si="10"/>
         <v>86.231249999999989</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AC9" s="1">
         <f>AVERAGE($D$8:$G$9)</f>
         <v>73.287499999999994</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AD9" s="1">
         <f t="shared" si="30"/>
         <v>73.287499999999994</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AE9" s="1">
         <f t="shared" si="30"/>
         <v>73.287499999999994</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AF9" s="1">
         <f t="shared" si="30"/>
         <v>73.287499999999994</v>
       </c>
-      <c r="AH9" s="2">
+      <c r="AH9" s="1">
         <f>AVERAGE($D$7:$G$7,$D$9:$G$9)</f>
         <v>70.5</v>
       </c>
-      <c r="AI9" s="2">
+      <c r="AI9" s="1">
         <f t="shared" ref="AI9:AK9" si="33">AVERAGE($D$7:$G$7,$D$9:$G$9)</f>
         <v>70.5</v>
       </c>
-      <c r="AJ9" s="2">
+      <c r="AJ9" s="1">
         <f t="shared" si="33"/>
         <v>70.5</v>
       </c>
-      <c r="AK9" s="2">
+      <c r="AK9" s="1">
         <f t="shared" si="33"/>
         <v>70.5</v>
       </c>
-      <c r="AM9" s="2">
+      <c r="AM9" s="1">
         <f>AVERAGE($D$5:$G$5,$D$9:$G$9)</f>
         <v>76.862499999999997</v>
       </c>
-      <c r="AN9" s="2">
+      <c r="AN9" s="1">
         <f t="shared" ref="AN9:AP9" si="34">AVERAGE($D$5:$G$5,$D$9:$G$9)</f>
         <v>76.862499999999997</v>
       </c>
-      <c r="AO9" s="2">
+      <c r="AO9" s="1">
         <f t="shared" si="34"/>
         <v>76.862499999999997</v>
       </c>
-      <c r="AP9" s="2">
+      <c r="AP9" s="1">
         <f t="shared" si="34"/>
         <v>76.862499999999997</v>
       </c>
-      <c r="AR9" s="2">
+      <c r="AR9" s="1">
         <f t="shared" si="13"/>
         <v>61.05</v>
       </c>
-      <c r="AS9" s="2">
+      <c r="AS9" s="1">
         <f t="shared" si="7"/>
         <v>61.05</v>
       </c>
-      <c r="AT9" s="2">
+      <c r="AT9" s="1">
         <f t="shared" si="7"/>
         <v>61.05</v>
       </c>
-      <c r="AU9" s="2">
+      <c r="AU9" s="1">
         <f t="shared" si="7"/>
         <v>61.05</v>
       </c>
@@ -2236,1196 +2236,1196 @@
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <f>AVERAGE($D$2:$G$9)</f>
         <v>95.146875000000009</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <f t="shared" ref="J12:L12" si="35">AVERAGE($D$2:$G$9)</f>
         <v>95.146875000000009</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <f t="shared" si="35"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <f t="shared" si="35"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <f>N2-I12</f>
         <v>15.578125</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="1">
         <f t="shared" ref="O12:Q19" si="36">O2-J12</f>
         <v>15.578125</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="1">
         <f>S2-I12</f>
         <v>6.1031249999999773</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="1">
         <f t="shared" ref="T12:V19" si="37">T2-J12</f>
         <v>6.1031249999999773</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12" s="1">
         <f>X2-I12</f>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Y12" s="1">
         <f t="shared" ref="Y12:AA12" si="38">Y2-J12</f>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="Z12" s="1">
         <f t="shared" si="38"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AA12" s="1">
         <f t="shared" si="38"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AC12" s="1">
         <f>AC2-SUM(S12,N12,I12)</f>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AD12" s="1">
         <f t="shared" ref="AD12:AF12" si="39">AD2-SUM(T12,O12,J12)</f>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="AE12" s="1">
         <f t="shared" si="39"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AF12" s="2">
+      <c r="AF12" s="1">
         <f t="shared" si="39"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AH12" s="2">
+      <c r="AH12" s="1">
         <f>AH2-SUM(X12,N12,I12)</f>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="AI12" s="1">
         <f t="shared" ref="AI12:AK19" si="40">AI2-SUM(Y12,O12,J12)</f>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AJ12" s="2">
+      <c r="AJ12" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AK12" s="2">
+      <c r="AK12" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AM12" s="2">
+      <c r="AM12" s="1">
         <f>AM2-SUM(X12,S12,I12)</f>
         <v>-3.265625</v>
       </c>
-      <c r="AN12" s="2">
+      <c r="AN12" s="1">
         <f t="shared" ref="AN12:AP12" si="41">AN2-SUM(Y12,T12,J12)</f>
         <v>-3.265625</v>
       </c>
-      <c r="AO12" s="2">
+      <c r="AO12" s="1">
         <f t="shared" si="41"/>
         <v>-3.265625</v>
       </c>
-      <c r="AP12" s="2">
+      <c r="AP12" s="1">
         <f t="shared" si="41"/>
         <v>-3.265625</v>
       </c>
-      <c r="AR12" s="2">
+      <c r="AR12" s="1">
         <f>AR2-SUM(X12,S12,N12,I12)</f>
         <v>-3.6937499999999943</v>
       </c>
-      <c r="AS12" s="2">
+      <c r="AS12" s="1">
         <f t="shared" ref="AS12:AU12" si="42">AS2-SUM(Y12,T12,O12,J12)</f>
         <v>-3.6937499999999943</v>
       </c>
-      <c r="AT12" s="2">
+      <c r="AT12" s="1">
         <f t="shared" si="42"/>
         <v>-3.6937499999999943</v>
       </c>
-      <c r="AU12" s="2">
+      <c r="AU12" s="1">
         <f t="shared" si="42"/>
         <v>-3.6937499999999943</v>
       </c>
-      <c r="AW12" s="2">
+      <c r="AW12" s="1">
         <f>D2-SUM(I12,N12,S12,X12,AC12,AH12,AM12,AR12)</f>
         <v>5.8468750000000114</v>
       </c>
-      <c r="AX12" s="2">
+      <c r="AX12" s="1">
         <f t="shared" ref="AX12:AZ12" si="43">E2-SUM(J12,O12,T12,Y12,AD12,AI12,AN12,AS12)</f>
         <v>2.1468750000000085</v>
       </c>
-      <c r="AY12" s="2">
+      <c r="AY12" s="1">
         <f t="shared" si="43"/>
         <v>2.2468750000000171</v>
       </c>
-      <c r="AZ12" s="2">
+      <c r="AZ12" s="1">
         <f t="shared" si="43"/>
         <v>4.1468750000000085</v>
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <f t="shared" ref="I13:L19" si="44">AVERAGE($D$2:$G$9)</f>
         <v>95.146875000000009</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <f t="shared" ref="N13:N19" si="45">N3-I13</f>
         <v>15.578125</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13" s="1">
         <f t="shared" ref="S13:S19" si="46">S3-I13</f>
         <v>6.1031249999999773</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13" s="1">
         <f t="shared" ref="X13:X19" si="47">X3-I13</f>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Y13" s="1">
         <f t="shared" ref="Y13:Y19" si="48">Y3-J13</f>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="Z13" s="1">
         <f t="shared" ref="Z13:Z19" si="49">Z3-K13</f>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AA13" s="1">
         <f t="shared" ref="AA13:AA19" si="50">AA3-L13</f>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AC13" s="1">
         <f t="shared" ref="AC13:AC19" si="51">AC3-SUM(S13,N13,I13)</f>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AD13" s="1">
         <f t="shared" ref="AD13:AD19" si="52">AD3-SUM(T13,O13,J13)</f>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AE13" s="1">
         <f t="shared" ref="AE13:AE19" si="53">AE3-SUM(U13,P13,K13)</f>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AF13" s="1">
         <f t="shared" ref="AF13:AF19" si="54">AF3-SUM(V13,Q13,L13)</f>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AH13" s="2">
+      <c r="AH13" s="1">
         <f t="shared" ref="AH13:AH19" si="55">AH3-SUM(X13,N13,I13)</f>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="AI13" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AJ13" s="2">
+      <c r="AJ13" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AK13" s="2">
+      <c r="AK13" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="AM13" s="1">
         <f t="shared" ref="AM13:AM19" si="56">AM3-SUM(X13,S13,I13)</f>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="AN13" s="1">
         <f t="shared" ref="AN13:AN19" si="57">AN3-SUM(Y13,T13,J13)</f>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AO13" s="2">
+      <c r="AO13" s="1">
         <f t="shared" ref="AO13:AO19" si="58">AO3-SUM(Z13,U13,K13)</f>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AP13" s="2">
+      <c r="AP13" s="1">
         <f t="shared" ref="AP13:AP19" si="59">AP3-SUM(AA13,V13,L13)</f>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AR13" s="2">
+      <c r="AR13" s="1">
         <f t="shared" ref="AR13:AR19" si="60">AR3-SUM(X13,S13,N13,I13)</f>
         <v>3.3375000000000341</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AS13" s="1">
         <f t="shared" ref="AS13:AS19" si="61">AS3-SUM(Y13,T13,O13,J13)</f>
         <v>3.3375000000000341</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AT13" s="1">
         <f t="shared" ref="AT13:AT19" si="62">AT3-SUM(Z13,U13,P13,K13)</f>
         <v>3.3375000000000341</v>
       </c>
-      <c r="AU13" s="2">
+      <c r="AU13" s="1">
         <f t="shared" ref="AU13:AU19" si="63">AU3-SUM(AA13,V13,Q13,L13)</f>
         <v>3.3375000000000341</v>
       </c>
-      <c r="AW13" s="2">
+      <c r="AW13" s="1">
         <f t="shared" ref="AW13:AW19" si="64">D3-SUM(I13,N13,S13,X13,AC13,AH13,AM13,AR13)</f>
         <v>-1.7906250000000767</v>
       </c>
-      <c r="AX13" s="2">
+      <c r="AX13" s="1">
         <f t="shared" ref="AX13:AX19" si="65">E3-SUM(J13,O13,T13,Y13,AD13,AI13,AN13,AS13)</f>
         <v>-4.2906250000000767</v>
       </c>
-      <c r="AY13" s="2">
+      <c r="AY13" s="1">
         <f t="shared" ref="AY13:AY19" si="66">F3-SUM(K13,P13,U13,Z13,AE13,AJ13,AO13,AT13)</f>
         <v>-0.99062500000007958</v>
       </c>
-      <c r="AZ13" s="2">
+      <c r="AZ13" s="1">
         <f t="shared" ref="AZ13:AZ19" si="67">G3-SUM(L13,Q13,V13,AA13,AF13,AK13,AP13,AU13)</f>
         <v>-5.8906250000000853</v>
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="1">
         <f t="shared" si="45"/>
         <v>15.578125</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="R14" s="3" t="s">
+      <c r="R14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="1">
         <f t="shared" si="46"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="V14" s="2">
+      <c r="V14" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="W14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14" s="1">
         <f t="shared" si="47"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Y14" s="1">
         <f t="shared" si="48"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="Z14" s="1">
         <f t="shared" si="49"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AA14" s="1">
         <f t="shared" si="50"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AB14" s="3" t="s">
+      <c r="AB14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AC14" s="1">
         <f t="shared" si="51"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AD14" s="2">
+      <c r="AD14" s="1">
         <f t="shared" si="52"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AE14" s="1">
         <f t="shared" si="53"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AF14" s="2">
+      <c r="AF14" s="1">
         <f t="shared" si="54"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AG14" s="3" t="s">
+      <c r="AG14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AH14" s="2">
+      <c r="AH14" s="1">
         <f t="shared" si="55"/>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AI14" s="2">
+      <c r="AI14" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AJ14" s="2">
+      <c r="AJ14" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AK14" s="2">
+      <c r="AK14" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312500000001705</v>
       </c>
-      <c r="AL14" s="3" t="s">
+      <c r="AL14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AM14" s="2">
+      <c r="AM14" s="1">
         <f t="shared" si="56"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AN14" s="2">
+      <c r="AN14" s="1">
         <f t="shared" si="57"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AO14" s="2">
+      <c r="AO14" s="1">
         <f t="shared" si="58"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AP14" s="2">
+      <c r="AP14" s="1">
         <f t="shared" si="59"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AQ14" s="3" t="s">
+      <c r="AQ14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AR14" s="2">
+      <c r="AR14" s="1">
         <f t="shared" si="60"/>
         <v>3.3875000000000171</v>
       </c>
-      <c r="AS14" s="2">
+      <c r="AS14" s="1">
         <f t="shared" si="61"/>
         <v>3.3875000000000171</v>
       </c>
-      <c r="AT14" s="2">
+      <c r="AT14" s="1">
         <f t="shared" si="62"/>
         <v>3.3875000000000171</v>
       </c>
-      <c r="AU14" s="2">
+      <c r="AU14" s="1">
         <f t="shared" si="63"/>
         <v>3.3875000000000171</v>
       </c>
-      <c r="AV14" s="3" t="s">
+      <c r="AV14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AW14" s="2">
+      <c r="AW14" s="1">
         <f t="shared" si="64"/>
         <v>-5.1156250000000227</v>
       </c>
-      <c r="AX14" s="2">
+      <c r="AX14" s="1">
         <f t="shared" si="65"/>
         <v>-0.31562500000001137</v>
       </c>
-      <c r="AY14" s="2">
+      <c r="AY14" s="1">
         <f t="shared" si="66"/>
         <v>-4.8156250000000114</v>
       </c>
-      <c r="AZ14" s="2">
+      <c r="AZ14" s="1">
         <f t="shared" si="67"/>
         <v>-2.9156250000000199</v>
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="1">
         <f t="shared" si="45"/>
         <v>15.578125</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="1">
         <f t="shared" si="36"/>
         <v>15.578125</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="1">
         <f t="shared" si="46"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15" s="1">
         <f t="shared" si="47"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Y15" s="1">
         <f t="shared" si="48"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="Z15" s="1">
         <f t="shared" si="49"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AA15" s="1">
         <f t="shared" si="50"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AC15" s="1">
         <f t="shared" si="51"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AD15" s="2">
+      <c r="AD15" s="1">
         <f t="shared" si="52"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AE15" s="1">
         <f t="shared" si="53"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="AF15" s="1">
         <f t="shared" si="54"/>
         <v>0.17812500000000853</v>
       </c>
-      <c r="AH15" s="2">
+      <c r="AH15" s="1">
         <f t="shared" si="55"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="AI15" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="AJ15" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AK15" s="2">
+      <c r="AK15" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AM15" s="2">
+      <c r="AM15" s="1">
         <f t="shared" si="56"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AN15" s="2">
+      <c r="AN15" s="1">
         <f t="shared" si="57"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AO15" s="2">
+      <c r="AO15" s="1">
         <f t="shared" si="58"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AP15" s="2">
+      <c r="AP15" s="1">
         <f t="shared" si="59"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AR15" s="2">
+      <c r="AR15" s="1">
         <f t="shared" si="60"/>
         <v>-3.0312499999999574</v>
       </c>
-      <c r="AS15" s="2">
+      <c r="AS15" s="1">
         <f t="shared" si="61"/>
         <v>-3.0312499999999574</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AT15" s="1">
         <f t="shared" si="62"/>
         <v>-3.0312499999999574</v>
       </c>
-      <c r="AU15" s="2">
+      <c r="AU15" s="1">
         <f t="shared" si="63"/>
         <v>-3.0312499999999574</v>
       </c>
-      <c r="AW15" s="2">
+      <c r="AW15" s="1">
         <f t="shared" si="64"/>
         <v>-1.5406250000000625</v>
       </c>
-      <c r="AX15" s="2">
+      <c r="AX15" s="1">
         <f t="shared" si="65"/>
         <v>6.2593749999999346</v>
       </c>
-      <c r="AY15" s="2">
+      <c r="AY15" s="1">
         <f t="shared" si="66"/>
         <v>6.6593749999999403</v>
       </c>
-      <c r="AZ15" s="2">
+      <c r="AZ15" s="1">
         <f t="shared" si="67"/>
         <v>0.35937499999992895</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="1">
         <f t="shared" si="45"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="1">
         <f t="shared" si="46"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V16" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16" s="1">
         <f t="shared" si="47"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Y16" s="1">
         <f t="shared" si="48"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="Z16" s="1">
         <f t="shared" si="49"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AA16" s="1">
         <f t="shared" si="50"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AC16" s="1">
         <f t="shared" si="51"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AD16" s="1">
         <f t="shared" si="52"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AE16" s="1">
         <f t="shared" si="53"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="AF16" s="1">
         <f t="shared" si="54"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AH16" s="2">
+      <c r="AH16" s="1">
         <f t="shared" si="55"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AI16" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AJ16" s="2">
+      <c r="AJ16" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AK16" s="2">
+      <c r="AK16" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="AM16" s="1">
         <f t="shared" si="56"/>
         <v>-3.265625</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="AN16" s="1">
         <f t="shared" si="57"/>
         <v>-3.265625</v>
       </c>
-      <c r="AO16" s="2">
+      <c r="AO16" s="1">
         <f t="shared" si="58"/>
         <v>-3.265625</v>
       </c>
-      <c r="AP16" s="2">
+      <c r="AP16" s="1">
         <f t="shared" si="59"/>
         <v>-3.265625</v>
       </c>
-      <c r="AR16" s="2">
+      <c r="AR16" s="1">
         <f t="shared" si="60"/>
         <v>-2.8374999999999631</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AS16" s="1">
         <f t="shared" si="61"/>
         <v>-2.8374999999999631</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AT16" s="1">
         <f t="shared" si="62"/>
         <v>-2.8374999999999631</v>
       </c>
-      <c r="AU16" s="2">
+      <c r="AU16" s="1">
         <f t="shared" si="63"/>
         <v>-2.8374999999999631</v>
       </c>
-      <c r="AW16" s="2">
+      <c r="AW16" s="1">
         <f t="shared" si="64"/>
         <v>2.0843749999999517</v>
       </c>
-      <c r="AX16" s="2">
+      <c r="AX16" s="1">
         <f t="shared" si="65"/>
         <v>6.4843749999999432</v>
       </c>
-      <c r="AY16" s="2">
+      <c r="AY16" s="1">
         <f t="shared" si="66"/>
         <v>-1.5625000000056843E-2</v>
       </c>
-      <c r="AZ16" s="2">
+      <c r="AZ16" s="1">
         <f t="shared" si="67"/>
         <v>3.184374999999946</v>
       </c>
     </row>
     <row r="17" spans="9:52" x14ac:dyDescent="0.25">
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="1">
         <f t="shared" si="45"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="Q17" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17" s="1">
         <f t="shared" si="46"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U17" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="V17" s="2">
+      <c r="V17" s="1">
         <f t="shared" si="37"/>
         <v>6.1031249999999773</v>
       </c>
-      <c r="X17" s="2">
+      <c r="X17" s="1">
         <f t="shared" si="47"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Y17" s="1">
         <f t="shared" si="48"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="Z17" s="1">
         <f t="shared" si="49"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AA17" s="1">
         <f t="shared" si="50"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AC17" s="2">
+      <c r="AC17" s="1">
         <f t="shared" si="51"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AD17" s="2">
+      <c r="AD17" s="1">
         <f t="shared" si="52"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AE17" s="2">
+      <c r="AE17" s="1">
         <f t="shared" si="53"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AF17" s="2">
+      <c r="AF17" s="1">
         <f t="shared" si="54"/>
         <v>0.17812500000003695</v>
       </c>
-      <c r="AH17" s="2">
+      <c r="AH17" s="1">
         <f t="shared" si="55"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AI17" s="2">
+      <c r="AI17" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AJ17" s="2">
+      <c r="AJ17" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AK17" s="2">
+      <c r="AK17" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AM17" s="2">
+      <c r="AM17" s="1">
         <f t="shared" si="56"/>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AN17" s="2">
+      <c r="AN17" s="1">
         <f t="shared" si="57"/>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AO17" s="2">
+      <c r="AO17" s="1">
         <f t="shared" si="58"/>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AP17" s="2">
+      <c r="AP17" s="1">
         <f t="shared" si="59"/>
         <v>3.2656250000000426</v>
       </c>
-      <c r="AR17" s="2">
+      <c r="AR17" s="1">
         <f t="shared" si="60"/>
         <v>3.1937500000000369</v>
       </c>
-      <c r="AS17" s="2">
+      <c r="AS17" s="1">
         <f t="shared" si="61"/>
         <v>3.1937500000000369</v>
       </c>
-      <c r="AT17" s="2">
+      <c r="AT17" s="1">
         <f t="shared" si="62"/>
         <v>3.1937500000000369</v>
       </c>
-      <c r="AU17" s="2">
+      <c r="AU17" s="1">
         <f t="shared" si="63"/>
         <v>3.1937500000000369</v>
       </c>
-      <c r="AW17" s="2">
+      <c r="AW17" s="1">
         <f t="shared" si="64"/>
         <v>-4.6406250000000995</v>
       </c>
-      <c r="AX17" s="2">
+      <c r="AX17" s="1">
         <f t="shared" si="65"/>
         <v>-2.6406250000000995</v>
       </c>
-      <c r="AY17" s="2">
+      <c r="AY17" s="1">
         <f t="shared" si="66"/>
         <v>0.25937499999990621</v>
       </c>
-      <c r="AZ17" s="2">
+      <c r="AZ17" s="1">
         <f t="shared" si="67"/>
         <v>-6.1406250000000995</v>
       </c>
     </row>
     <row r="18" spans="9:52" x14ac:dyDescent="0.25">
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="1">
         <f t="shared" si="45"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18" s="1">
         <f t="shared" si="46"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U18" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="V18" s="2">
+      <c r="V18" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="X18" s="2">
+      <c r="X18" s="1">
         <f t="shared" si="47"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Y18" s="1">
         <f t="shared" si="48"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="Z18" s="1">
         <f t="shared" si="49"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AA18" s="1">
         <f t="shared" si="50"/>
         <v>8.9156249999999915</v>
       </c>
-      <c r="AC18" s="2">
+      <c r="AC18" s="1">
         <f t="shared" si="51"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AD18" s="2">
+      <c r="AD18" s="1">
         <f t="shared" si="52"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AE18" s="2">
+      <c r="AE18" s="1">
         <f t="shared" si="53"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AF18" s="2">
+      <c r="AF18" s="1">
         <f t="shared" si="54"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AH18" s="2">
+      <c r="AH18" s="1">
         <f t="shared" si="55"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AI18" s="2">
+      <c r="AI18" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AJ18" s="2">
+      <c r="AJ18" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AK18" s="2">
+      <c r="AK18" s="1">
         <f t="shared" si="40"/>
         <v>0.15312500000001705</v>
       </c>
-      <c r="AM18" s="2">
+      <c r="AM18" s="1">
         <f t="shared" si="56"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AN18" s="2">
+      <c r="AN18" s="1">
         <f t="shared" si="57"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AO18" s="2">
+      <c r="AO18" s="1">
         <f t="shared" si="58"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AP18" s="2">
+      <c r="AP18" s="1">
         <f t="shared" si="59"/>
         <v>3.2656250000000284</v>
       </c>
-      <c r="AR18" s="2">
+      <c r="AR18" s="1">
         <f t="shared" si="60"/>
         <v>3.1437500000000256</v>
       </c>
-      <c r="AS18" s="2">
+      <c r="AS18" s="1">
         <f t="shared" si="61"/>
         <v>3.1437500000000256</v>
       </c>
-      <c r="AT18" s="2">
+      <c r="AT18" s="1">
         <f t="shared" si="62"/>
         <v>3.1437500000000256</v>
       </c>
-      <c r="AU18" s="2">
+      <c r="AU18" s="1">
         <f t="shared" si="63"/>
         <v>3.1437500000000256</v>
       </c>
-      <c r="AW18" s="2">
+      <c r="AW18" s="1">
         <f t="shared" si="64"/>
         <v>1.1343749999999488</v>
       </c>
-      <c r="AX18" s="2">
+      <c r="AX18" s="1">
         <f t="shared" si="65"/>
         <v>-5.7656250000000568</v>
       </c>
-      <c r="AY18" s="2">
+      <c r="AY18" s="1">
         <f t="shared" si="66"/>
         <v>-2.2656250000000568</v>
       </c>
-      <c r="AZ18" s="2">
+      <c r="AZ18" s="1">
         <f t="shared" si="67"/>
         <v>-6.065625000000054</v>
       </c>
     </row>
     <row r="19" spans="9:52" x14ac:dyDescent="0.25">
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="1">
         <f t="shared" si="44"/>
         <v>95.146875000000009</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="1">
         <f t="shared" si="45"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q19" s="1">
         <f t="shared" si="36"/>
         <v>-15.578125000000014</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19" s="1">
         <f t="shared" si="46"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U19" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="V19" s="2">
+      <c r="V19" s="1">
         <f t="shared" si="37"/>
         <v>-6.1031250000000199</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X19" s="1">
         <f t="shared" si="47"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Y19" s="1">
         <f t="shared" si="48"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="Z19" s="1">
         <f t="shared" si="49"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AA19" s="1">
         <f t="shared" si="50"/>
         <v>-8.9156250000000199</v>
       </c>
-      <c r="AC19" s="2">
+      <c r="AC19" s="1">
         <f t="shared" si="51"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AD19" s="2">
+      <c r="AD19" s="1">
         <f t="shared" si="52"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AE19" s="2">
+      <c r="AE19" s="1">
         <f t="shared" si="53"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AF19" s="2">
+      <c r="AF19" s="1">
         <f t="shared" si="54"/>
         <v>-0.1781249999999801</v>
       </c>
-      <c r="AH19" s="2">
+      <c r="AH19" s="1">
         <f t="shared" si="55"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AI19" s="2">
+      <c r="AI19" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AJ19" s="2">
+      <c r="AJ19" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AK19" s="2">
+      <c r="AK19" s="1">
         <f t="shared" si="40"/>
         <v>-0.15312499999997442</v>
       </c>
-      <c r="AM19" s="2">
+      <c r="AM19" s="1">
         <f t="shared" si="56"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AN19" s="2">
+      <c r="AN19" s="1">
         <f t="shared" si="57"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AO19" s="2">
+      <c r="AO19" s="1">
         <f t="shared" si="58"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AP19" s="2">
+      <c r="AP19" s="1">
         <f t="shared" si="59"/>
         <v>-3.2656249999999716</v>
       </c>
-      <c r="AR19" s="2">
+      <c r="AR19" s="1">
         <f t="shared" si="60"/>
         <v>-3.4999999999999574</v>
       </c>
-      <c r="AS19" s="2">
+      <c r="AS19" s="1">
         <f t="shared" si="61"/>
         <v>-3.4999999999999574</v>
       </c>
-      <c r="AT19" s="2">
+      <c r="AT19" s="1">
         <f t="shared" si="62"/>
         <v>-3.4999999999999574</v>
       </c>
-      <c r="AU19" s="2">
+      <c r="AU19" s="1">
         <f t="shared" si="63"/>
         <v>-3.4999999999999574</v>
       </c>
-      <c r="AW19" s="2">
+      <c r="AW19" s="1">
         <f t="shared" si="64"/>
         <v>1.1468749999999304</v>
       </c>
-      <c r="AX19" s="2">
+      <c r="AX19" s="1">
         <f t="shared" si="65"/>
         <v>6.0468749999999289</v>
       </c>
-      <c r="AY19" s="2">
+      <c r="AY19" s="1">
         <f t="shared" si="66"/>
         <v>2.3468749999999261</v>
       </c>
-      <c r="AZ19" s="2">
+      <c r="AZ19" s="1">
         <f t="shared" si="67"/>
         <v>4.8468749999999261</v>
       </c>

</xml_diff>